<commit_message>
more modular, settings file, train and test sets more accurated
</commit_message>
<xml_diff>
--- a/scripts/mimic-iii/files/results.xlsx
+++ b/scripts/mimic-iii/files/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruna/Desktop/Bruna/UFMG/Dissertation/repos/fairness-ml-health/scripts/mimic-iii/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5192FA-C307-1444-8F14-39AA130F6ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38818010-5E63-FA4B-8B4B-C496C08BB7AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25260" windowHeight="14460" xr2:uid="{7DF2F523-AE6B-1340-A634-5252C1F719EC}"/>
+    <workbookView xWindow="12600" yWindow="460" windowWidth="13000" windowHeight="14460" xr2:uid="{7DF2F523-AE6B-1340-A634-5252C1F719EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>MLP</t>
   </si>
@@ -53,9 +53,6 @@
     <t>DeepHit</t>
   </si>
   <si>
-    <t>Brier</t>
-  </si>
-  <si>
     <t>Binomial Log-Likelihood</t>
   </si>
   <si>
@@ -75,6 +72,15 @@
   </si>
   <si>
     <t>RSF v1</t>
+  </si>
+  <si>
+    <t>Validação</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Brier *</t>
   </si>
 </sst>
 </file>
@@ -110,11 +116,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E8543E-1D4F-7A40-A262-2D8A929C83EF}">
-  <dimension ref="A3:F14"/>
+  <dimension ref="A3:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:E14"/>
+      <selection activeCell="C16" sqref="C16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,27 +448,33 @@
     <col min="4" max="4" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -474,8 +487,14 @@
       <c r="F5">
         <v>1821</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>9101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -488,10 +507,16 @@
       <c r="F6">
         <v>1821</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>9101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>0.71948999999999996</v>
@@ -502,10 +527,16 @@
       <c r="F7">
         <v>1821</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>9101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8">
         <v>7280</v>
@@ -513,8 +544,14 @@
       <c r="F8">
         <v>1821</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>9101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -527,8 +564,20 @@
       <c r="D9">
         <v>0.47061999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>5824</v>
+      </c>
+      <c r="F9">
+        <v>1821</v>
+      </c>
+      <c r="G9">
+        <v>1456</v>
+      </c>
+      <c r="H9">
+        <v>9101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -541,8 +590,20 @@
       <c r="D10">
         <v>0.48183999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>5824</v>
+      </c>
+      <c r="F10">
+        <v>1821</v>
+      </c>
+      <c r="G10">
+        <v>1456</v>
+      </c>
+      <c r="H10">
+        <v>9101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -555,8 +616,20 @@
       <c r="D11">
         <v>1.52356</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>5824</v>
+      </c>
+      <c r="F11">
+        <v>1821</v>
+      </c>
+      <c r="G11">
+        <v>1456</v>
+      </c>
+      <c r="H11">
+        <v>9101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -569,17 +642,43 @@
       <c r="D12">
         <v>0.48264000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E12">
+        <v>5824</v>
+      </c>
+      <c r="F12">
+        <v>1821</v>
+      </c>
+      <c r="G12">
+        <v>1456</v>
+      </c>
+      <c r="H12">
+        <v>9101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E13" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C16:E16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>